<commit_message>
First working cut of Ground_to_Water.py, update to well_dimensions
-[] Ground_to_Water.py produces averaged ground_to_water_cm measurement, verified on random entries; not yet fully featured
-[] updated well_dimensions.csv and .xlsx to fix bad dates for A1N and A2N
-[] groundwater_biweekly_FULL.csv produced by Ground_to_Water.py has 1117 entries for 54 wells in 2018, 2019, 2021.
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/well_dimensions.xlsx
+++ b/data/field_observations/groundwater/well_dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SANDISK_SSD_G40/GoogleDrive/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C09363-1239-634F-A3D9-010C278A385B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5BBE6DB-AC1F-0444-B44E-475EFBF0202D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="520" windowWidth="34480" windowHeight="21320" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
+    <workbookView xWindow="25820" yWindow="680" windowWidth="13480" windowHeight="21160" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="well_dimensions" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="14">
-        <v>45413.375</v>
+        <v>43250.375</v>
       </c>
       <c r="D13" s="14">
         <v>45571.5</v>
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="14">
-        <v>45413.375</v>
+        <v>43250.375</v>
       </c>
       <c r="D15" s="14">
         <v>45571.5</v>

</xml_diff>

<commit_message>
validated all bi-weekly groundwater data and created MARSS R script
- Added all 2024 groundwater data (except Lo wells on 11/09/2024)
- Validated all individual well plots
- noted issues and changes in  well_data_vaildation_steps.csv
- Created MARSS_Sagehen_Groundwater.R script with stubbed out functions
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/well_dimensions.xlsx
+++ b/data/field_observations/groundwater/well_dimensions.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SANDISK_SSD_G40/GoogleDrive/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5BBE6DB-AC1F-0444-B44E-475EFBF0202D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE1C07E-0731-2B49-8F20-12723415DB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25820" yWindow="680" windowWidth="13480" windowHeight="21160" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
+    <workbookView xWindow="1660" yWindow="3760" windowWidth="27180" windowHeight="18360" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="well_dimensions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="162">
   <si>
     <t>well_id</t>
   </si>
@@ -70,9 +84,6 @@
     <t>EFF-XA2N</t>
   </si>
   <si>
-    <t>EFF-XB7S</t>
-  </si>
-  <si>
     <t>EFR-XB1S</t>
   </si>
   <si>
@@ -91,9 +102,6 @@
     <t>EFR-XB3S</t>
   </si>
   <si>
-    <t>EFT-XB6S</t>
-  </si>
-  <si>
     <t>EHF-XA3S</t>
   </si>
   <si>
@@ -106,9 +114,6 @@
     <t>EHT-XA5S</t>
   </si>
   <si>
-    <t>EET-XB4S</t>
-  </si>
-  <si>
     <t>EHT-XB5S</t>
   </si>
   <si>
@@ -491,17 +496,42 @@
   </si>
   <si>
     <t>new well installed on 07/05/2019 (orange p71); ignore because no well depth</t>
+  </si>
+  <si>
+    <t>from 11/09/2024: in canopy of two pine trees (one alive, one dead), otherwise MH; on a terrace that butts up against the creek, looks like a big drop to the creek such that there's no floodplain on this side of the creek.</t>
+  </si>
+  <si>
+    <t>from 11/09/2024: def pine, def terrace (same one as C3S)</t>
+  </si>
+  <si>
+    <t>EHF-XB7S</t>
+  </si>
+  <si>
+    <t>from 11/09/2024: MH and probably terrace, not currrently in pine canopy, but small pines close just no canopy over well</t>
+  </si>
+  <si>
+    <t>EHT-XB6S</t>
+  </si>
+  <si>
+    <t>from 10/20/2024: MH, no pine canopy covering well, closest pine is 0.95 m away (trunk is ~10cm and trunk is 2.75 m away); otherwise dead pines on ground</t>
+  </si>
+  <si>
+    <t>EER-XB4S</t>
+  </si>
+  <si>
+    <t>from 11/09/2024: kind of on edge between terrace and riparian but it's downslope from B5S terrace; interesting to analyze topo from LiDAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -653,6 +683,13 @@
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -989,7 +1026,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1032,8 +1069,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1063,16 +1101,16 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="4" xfId="9" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="36" borderId="4" xfId="9" applyFill="1"/>
-    <xf numFmtId="171" fontId="9" fillId="33" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="33" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="35" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="35" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1082,7 +1120,7 @@
     <xf numFmtId="0" fontId="20" fillId="37" borderId="4" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="37" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="37" borderId="4" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="37" borderId="4" xfId="9" applyFill="1"/>
@@ -1092,42 +1130,27 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="20" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="4" xfId="9" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="4" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="4" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="34" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="4" xfId="9" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="4" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="37" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="4" xfId="9" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="38" borderId="4" xfId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="20" fillId="37" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="37" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="4" xfId="9" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="4" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1155,6 +1178,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1505,7 +1529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1529,19 +1553,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -1556,25 +1580,25 @@
         <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1597,14 +1621,14 @@
         <v>154.4</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O2" s="3"/>
     </row>
@@ -1628,7 +1652,7 @@
         <v>154.02500000000001</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1655,10 +1679,10 @@
         <v>155</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1685,16 +1709,16 @@
         <v>156.19999999999999</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1717,25 +1741,25 @@
         <v>149.15</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M6" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="17" t="s">
-        <v>81</v>
-      </c>
       <c r="O6" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1758,7 +1782,7 @@
         <v>147</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1782,14 +1806,14 @@
         <v>12.824999999999999</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1812,24 +1836,24 @@
         <v>154.69999999999999</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="N9" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="B10" s="18" t="b">
         <v>1</v>
@@ -1847,20 +1871,25 @@
         <v>146.5</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="O10" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="P10" s="25" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="11" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="B11" s="18" t="b">
         <v>1</v>
@@ -1878,7 +1907,7 @@
         <v>152</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
@@ -1902,24 +1931,24 @@
         <v>99.325000000000003</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="7" t="b">
@@ -1938,22 +1967,22 @@
         <v>100</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="N13" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="O13" s="33" t="s">
-        <v>78</v>
+        <v>37</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1973,14 +2002,14 @@
         <v>44.524099999999997</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
       <c r="P14" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2003,27 +2032,27 @@
         <v>153</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="B16" s="18" t="b">
         <v>1</v>
@@ -2041,16 +2070,27 @@
         <v>153.13</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="17" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="B17" s="18" t="b">
         <v>1</v>
@@ -2068,7 +2108,7 @@
         <v>152.80000000000001</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -2077,7 +2117,7 @@
     </row>
     <row r="18" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="18" t="b">
         <v>1</v>
@@ -2095,16 +2135,24 @@
         <v>153.19999999999999</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="19" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="18" t="b">
         <v>1</v>
@@ -2122,19 +2170,19 @@
         <v>153.80000000000001</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="18" t="b">
         <v>1</v>
@@ -2152,7 +2200,7 @@
         <v>156.30000000000001</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
@@ -2161,7 +2209,7 @@
     </row>
     <row r="21" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="18" t="b">
         <v>1</v>
@@ -2179,27 +2227,27 @@
         <v>156.30000000000001</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M21" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N21" s="26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O21" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="22" t="b">
         <v>0</v>
@@ -2214,16 +2262,24 @@
         <v>116</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="22" t="b">
         <v>0</v>
@@ -2238,7 +2294,7 @@
         <v>116.65</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
@@ -2247,7 +2303,7 @@
     </row>
     <row r="24" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="7" t="b">
         <v>1</v>
@@ -2265,19 +2321,19 @@
         <v>153.36670000000001</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="7" t="b">
         <v>1</v>
@@ -2295,7 +2351,7 @@
         <v>153.5</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -2304,7 +2360,7 @@
     </row>
     <row r="26" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7" t="b">
         <v>1</v>
@@ -2322,7 +2378,7 @@
         <v>152.833</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -2331,7 +2387,7 @@
     </row>
     <row r="27" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="7" t="b">
         <v>1</v>
@@ -2349,16 +2405,24 @@
         <v>152.80000000000001</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="B28" s="18" t="b">
         <v>1</v>
@@ -2376,16 +2440,27 @@
         <v>152.69999999999999</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="O28" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="29" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="B29" s="18" t="b">
         <v>1</v>
@@ -2403,7 +2478,7 @@
         <v>152.30000000000001</v>
       </c>
       <c r="K29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
@@ -2430,12 +2505,23 @@
         <v>152.80000000000001</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="31" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
@@ -2457,16 +2543,27 @@
         <v>147.80000000000001</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="32" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="18" t="b">
         <v>1</v>
@@ -2484,43 +2581,43 @@
         <v>132.80000000000001</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="18"/>
     </row>
-    <row r="33" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="28">
         <v>44393.5</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="28">
         <v>44396.5</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="29">
         <v>59.65</v>
       </c>
-      <c r="K33" s="35" t="s">
-        <v>67</v>
+      <c r="K33" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="35" t="s">
-        <v>142</v>
+      <c r="P33" s="29" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
-        <v>24</v>
+      <c r="A34" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="B34" s="7" t="b">
         <v>1</v>
@@ -2538,27 +2635,27 @@
         <v>155</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="L34" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M34" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="M34" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="N34" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="O34" s="33" t="s">
-        <v>80</v>
+      <c r="N34" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" s="22" t="b">
         <v>0</v>
@@ -2573,19 +2670,19 @@
         <v>54.789000000000001</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
       <c r="P35" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B36" s="7" t="b">
         <v>1</v>
@@ -2603,24 +2700,24 @@
         <v>154.4</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O36" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B37" s="7" t="b">
         <v>1</v>
@@ -2638,19 +2735,19 @@
         <v>155.4</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
       <c r="P37" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B38" s="22" t="b">
         <v>0</v>
@@ -2668,19 +2765,19 @@
         <v>155.4</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
       <c r="P38" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B39" s="7" t="b">
         <v>1</v>
@@ -2698,130 +2795,130 @@
         <v>155.19999999999999</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P39" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="14">
+        <v>43250.375</v>
+      </c>
+      <c r="D40" s="14">
+        <v>43252.279861111114</v>
+      </c>
+      <c r="E40" s="9">
+        <v>38.337499999999999</v>
+      </c>
+      <c r="G40" s="9">
+        <v>145.33333329999999</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="14">
+        <v>44393.208333333336</v>
+      </c>
+      <c r="D41" s="14">
+        <v>44393.5</v>
+      </c>
+      <c r="E41" s="9">
+        <v>27.318750000000001</v>
+      </c>
+      <c r="G41" s="9">
+        <v>154.5</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N41" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="N39" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O39" s="7" t="s">
+      <c r="O41" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="20">
+        <v>45413.375</v>
+      </c>
+      <c r="D42" s="20">
+        <v>45571.5</v>
+      </c>
+      <c r="E42" s="21">
+        <v>27.75</v>
+      </c>
+      <c r="K42" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="L42" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="M42" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="N42" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="P39" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C40" s="28">
-        <v>43250.375</v>
-      </c>
-      <c r="D40" s="28">
-        <v>43252.279861111114</v>
-      </c>
-      <c r="E40" s="29">
-        <v>38.337499999999999</v>
-      </c>
-      <c r="G40" s="29">
-        <v>145.33333329999999</v>
-      </c>
-      <c r="K40" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41" s="28">
-        <v>44393.208333333336</v>
-      </c>
-      <c r="D41" s="28">
-        <v>44393.5</v>
-      </c>
-      <c r="E41" s="29">
-        <v>27.318750000000001</v>
-      </c>
-      <c r="G41" s="29">
-        <v>154.5</v>
-      </c>
-      <c r="K41" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="N41" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="O41" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="P41" s="29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" s="31">
-        <v>45413.375</v>
-      </c>
-      <c r="D42" s="31">
-        <v>45571.5</v>
-      </c>
-      <c r="E42" s="32">
-        <v>27.75</v>
-      </c>
-      <c r="K42" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="L42" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M42" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="N42" s="23" t="s">
-        <v>81</v>
-      </c>
       <c r="O42" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="P42" s="32" t="s">
-        <v>129</v>
+        <v>93</v>
+      </c>
+      <c r="P42" s="21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B43" s="22" t="b">
         <v>0</v>
@@ -2836,19 +2933,19 @@
         <v>152.94999999999999</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
       <c r="P43" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B44" s="7" t="b">
         <v>1</v>
@@ -2866,7 +2963,7 @@
         <v>153.667</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
@@ -2875,7 +2972,7 @@
     </row>
     <row r="45" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B45" s="7" t="b">
         <v>1</v>
@@ -2893,7 +2990,7 @@
         <v>153.19999999999999</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
@@ -2920,19 +3017,27 @@
         <v>152.69999999999999</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="P46" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B47" s="7" t="b">
         <v>1</v>
@@ -2950,7 +3055,7 @@
         <v>152.08250000000001</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
@@ -2959,7 +3064,7 @@
     </row>
     <row r="48" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B48" s="7" t="b">
         <v>1</v>
@@ -2977,92 +3082,92 @@
         <v>153</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M48" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N48" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="N48" s="7" t="s">
+      <c r="O48" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P48" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" s="14">
+        <v>43250.375</v>
+      </c>
+      <c r="D49" s="14">
+        <v>43252.26666666667</v>
+      </c>
+      <c r="E49" s="9">
+        <v>95.064499999999995</v>
+      </c>
+      <c r="G49" s="9">
+        <v>149.53299999999999</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="14">
+        <v>44393.5</v>
+      </c>
+      <c r="D50" s="14">
+        <v>45571.5</v>
+      </c>
+      <c r="E50" s="9">
+        <v>85.606250000000003</v>
+      </c>
+      <c r="G50" s="9">
+        <v>130</v>
+      </c>
+      <c r="K50" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L50" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="O48" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="P48" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" s="28">
-        <v>43250.375</v>
-      </c>
-      <c r="D49" s="28">
-        <v>43252.26666666667</v>
-      </c>
-      <c r="E49" s="29">
-        <v>95.064499999999995</v>
-      </c>
-      <c r="G49" s="29">
-        <v>149.53299999999999</v>
-      </c>
-      <c r="K49" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="27"/>
-    </row>
-    <row r="50" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" s="28">
-        <v>44393.5</v>
-      </c>
-      <c r="D50" s="28">
-        <v>45571.5</v>
-      </c>
-      <c r="E50" s="29">
-        <v>85.606250000000003</v>
-      </c>
-      <c r="G50" s="29">
-        <v>130</v>
-      </c>
-      <c r="K50" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L50" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="M50" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="N50" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="O50" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="P50" s="29" t="s">
-        <v>144</v>
+      <c r="M50" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="N50" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="O50" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="P50" s="9" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B51" s="7" t="b">
         <v>1</v>
@@ -3080,22 +3185,22 @@
         <v>131.5</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
       <c r="P51" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B52" s="7" t="b">
         <v>1</v>
@@ -3113,27 +3218,27 @@
         <v>111.2</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M52" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N52" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P52" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53" s="7" t="b">
         <v>1</v>
@@ -3151,7 +3256,7 @@
         <v>155.1</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
@@ -3159,8 +3264,8 @@
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="33" t="s">
-        <v>21</v>
+      <c r="A54" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="B54" s="7" t="b">
         <v>1</v>
@@ -3178,27 +3283,27 @@
         <v>154.9</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L54" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="M54" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="N54" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="O54" s="33" t="s">
-        <v>80</v>
+        <v>37</v>
+      </c>
+      <c r="L54" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M54" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="O54" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="P54" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B55" s="7" t="b">
         <v>1</v>
@@ -3216,7 +3321,7 @@
         <v>154.80000000000001</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L55" s="7"/>
       <c r="M55" s="7"/>
@@ -3225,7 +3330,7 @@
     </row>
     <row r="56" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B56" s="7" t="b">
         <v>1</v>
@@ -3243,27 +3348,27 @@
         <v>154.5</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M56" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N56" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O56" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P56" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B57" s="18" t="b">
         <v>1</v>
@@ -3281,7 +3386,7 @@
         <v>149.9</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L57" s="18"/>
       <c r="M57" s="18"/>
@@ -3290,7 +3395,7 @@
     </row>
     <row r="58" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B58" s="18" t="b">
         <v>1</v>
@@ -3308,19 +3413,19 @@
         <v>152</v>
       </c>
       <c r="K58" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L58" s="18"/>
       <c r="M58" s="18"/>
       <c r="N58" s="18"/>
       <c r="O58" s="18"/>
       <c r="P58" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B59" s="18" t="b">
         <v>1</v>
@@ -3338,19 +3443,19 @@
         <v>216.5</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
       <c r="N59" s="18"/>
       <c r="O59" s="18"/>
       <c r="P59" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B60" s="18" t="b">
         <v>1</v>
@@ -3368,27 +3473,27 @@
         <v>216.5</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L60" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M60" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N60" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N60" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="O60" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P60" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B61" s="7" t="b">
         <v>1</v>
@@ -3406,7 +3511,7 @@
         <v>153.85</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
@@ -3415,7 +3520,7 @@
     </row>
     <row r="62" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B62" s="7" t="b">
         <v>1</v>
@@ -3433,27 +3538,27 @@
         <v>153.1</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M62" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N62" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O62" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P62" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B63" s="22" t="b">
         <v>0</v>
@@ -3471,27 +3576,27 @@
         <v>1976.422</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L63" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M63" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N63" s="22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O63" s="22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P63" s="21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B64" s="22" t="b">
         <v>0</v>
@@ -3506,19 +3611,19 @@
         <v>35.825000000000003</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L64" s="22"/>
       <c r="M64" s="22"/>
       <c r="N64" s="22"/>
       <c r="O64" s="22"/>
       <c r="P64" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B65" s="7" t="b">
         <v>1</v>
@@ -3537,24 +3642,24 @@
         <v>151.30000000000001</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N65" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O65" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B66" s="7" t="b">
         <v>1</v>
@@ -3572,19 +3677,19 @@
         <v>0</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
       <c r="P66" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B67" s="7" t="b">
         <v>1</v>
@@ -3602,19 +3707,19 @@
         <v>144.69999999999999</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
       <c r="P67" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B68" s="7" t="b">
         <v>1</v>
@@ -3632,19 +3737,19 @@
         <v>147</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
       <c r="P68" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B69" s="7" t="b">
         <v>1</v>
@@ -3663,27 +3768,27 @@
         <v>144.69999999999999</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M69" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N69" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O69" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P69" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B70" s="18" t="b">
         <v>1</v>
@@ -3701,10 +3806,10 @@
         <v>147.9</v>
       </c>
       <c r="J70" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K70" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L70" s="18"/>
       <c r="M70" s="18"/>
@@ -3713,7 +3818,7 @@
     </row>
     <row r="71" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B71" s="18" t="b">
         <v>1</v>
@@ -3732,27 +3837,27 @@
         <v>152.80000000000001</v>
       </c>
       <c r="K71" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L71" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M71" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N71" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N71" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="O71" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P71" s="25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B72" s="18" t="b">
         <v>1</v>
@@ -3770,30 +3875,30 @@
         <v>147.6</v>
       </c>
       <c r="J72" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K72" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L72" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M72" s="18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N72" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O72" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B73" s="18" t="b">
         <v>1</v>
@@ -3808,19 +3913,19 @@
         <v>0</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L73" s="18"/>
       <c r="M73" s="18"/>
       <c r="N73" s="18"/>
       <c r="O73" s="18"/>
       <c r="P73" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B74" s="18" t="b">
         <v>1</v>
@@ -3838,27 +3943,27 @@
         <v>142</v>
       </c>
       <c r="K74" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L74" s="26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M74" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="N74" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="O74" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="P74" s="25" t="s">
         <v>96</v>
-      </c>
-      <c r="N74" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="O74" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="P74" s="25" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B75" s="7" t="b">
         <v>1</v>
@@ -3876,10 +3981,10 @@
         <v>150.80000000000001</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -3888,7 +3993,7 @@
     </row>
     <row r="76" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B76" s="7" t="b">
         <v>1</v>
@@ -3909,24 +4014,24 @@
         <v>1981.3920000000001</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M76" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N76" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O76" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B77" s="22" t="b">
         <v>0</v>
@@ -3941,19 +4046,19 @@
         <v>60.697499999999998</v>
       </c>
       <c r="K77" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>
       <c r="N77" s="22"/>
       <c r="O77" s="22"/>
       <c r="P77" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B78" s="7" t="b">
         <v>1</v>
@@ -3977,24 +4082,24 @@
         <v>1982.229</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L78" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M78" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N78" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O78" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B79" s="18" t="b">
         <v>1</v>
@@ -4012,19 +4117,19 @@
         <v>148.85220000000001</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L79" s="18"/>
       <c r="M79" s="18"/>
       <c r="N79" s="18"/>
       <c r="O79" s="18"/>
       <c r="P79" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B80" s="18" t="b">
         <v>1</v>
@@ -4042,19 +4147,19 @@
         <v>163.80000000000001</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L80" s="18"/>
       <c r="M80" s="18"/>
       <c r="N80" s="18"/>
       <c r="O80" s="18"/>
       <c r="P80" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B81" s="18" t="b">
         <v>1</v>
@@ -4072,27 +4177,27 @@
         <v>201</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L81" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M81" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N81" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O81" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P81" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="33" t="s">
-        <v>47</v>
+      <c r="A82" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="B82" s="7" t="b">
         <v>1</v>
@@ -4110,27 +4215,27 @@
         <v>153.4</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L82" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="M82" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="N82" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="O82" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L82" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="M82" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="N82" s="27" t="s">
         <v>78</v>
       </c>
+      <c r="O82" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="P82" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B83" s="7" t="b">
         <v>1</v>
@@ -4148,7 +4253,7 @@
         <v>148.59</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
@@ -4157,7 +4262,7 @@
     </row>
     <row r="84" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B84" s="10" t="b">
         <v>0</v>
@@ -4177,12 +4282,12 @@
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
       <c r="P84" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B85" s="22" t="b">
         <v>0</v>
@@ -4197,19 +4302,19 @@
         <v>48.14</v>
       </c>
       <c r="K85" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L85" s="22"/>
       <c r="M85" s="22"/>
       <c r="N85" s="22"/>
       <c r="O85" s="22"/>
       <c r="P85" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B86" s="7" t="b">
         <v>1</v>
@@ -4228,27 +4333,27 @@
         <v>143.6</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M86" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N86" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O86" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P86" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B87" s="7" t="b">
         <v>1</v>
@@ -4269,27 +4374,27 @@
         <v>1976.1489999999999</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L87" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M87" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O87" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P87" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B88" s="7" t="b">
         <v>1</v>
@@ -4307,7 +4412,7 @@
         <v>137</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
@@ -4316,7 +4421,7 @@
     </row>
     <row r="89" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B89" s="18" t="b">
         <v>1</v>
@@ -4337,24 +4442,24 @@
         <v>1976.1859999999999</v>
       </c>
       <c r="K89" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L89" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M89" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N89" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O89" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B90" s="18" t="b">
         <v>1</v>
@@ -4372,7 +4477,7 @@
         <v>147.07</v>
       </c>
       <c r="K90" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L90" s="18"/>
       <c r="M90" s="18"/>
@@ -4381,7 +4486,7 @@
     </row>
     <row r="91" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B91" s="7" t="b">
         <v>1</v>
@@ -4399,19 +4504,19 @@
         <v>131</v>
       </c>
       <c r="K91" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L91" s="7"/>
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
       <c r="P91" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B92" s="22" t="b">
         <v>0</v>
@@ -4427,27 +4532,27 @@
         <v>56.25</v>
       </c>
       <c r="K92" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L92" s="22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M92" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N92" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O92" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B93" s="7" t="b">
         <v>1</v>
@@ -4465,19 +4570,19 @@
         <v>111</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L93" s="7"/>
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
       <c r="P93" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B94" s="7" t="b">
         <v>1</v>
@@ -4495,7 +4600,7 @@
         <v>150</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L94" s="7"/>
       <c r="M94" s="7"/>
@@ -4503,8 +4608,8 @@
       <c r="O94" s="7"/>
     </row>
     <row r="95" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="33" t="s">
-        <v>54</v>
+      <c r="A95" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="B95" s="7" t="b">
         <v>1</v>
@@ -4525,27 +4630,27 @@
         <v>1976.7739999999999</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L95" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="M95" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L95" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M95" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="N95" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="N95" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="O95" s="33" t="s">
-        <v>80</v>
+      <c r="O95" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="P95" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B96" s="7" t="b">
         <v>1</v>
@@ -4563,7 +4668,7 @@
         <v>142.25550000000001</v>
       </c>
       <c r="K96" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
@@ -4572,7 +4677,7 @@
     </row>
     <row r="97" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B97" s="7" t="b">
         <v>1</v>
@@ -4591,27 +4696,27 @@
         <v>226.5</v>
       </c>
       <c r="K97" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L97" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M97" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N97" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="N97" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="O97" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P97" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B98" s="7" t="b">
         <v>1</v>
@@ -4629,19 +4734,19 @@
         <v>142.125</v>
       </c>
       <c r="K98" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
       <c r="P98" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B99" s="7" t="b">
         <v>1</v>
@@ -4660,27 +4765,27 @@
         <v>139.80000000000001</v>
       </c>
       <c r="K99" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L99" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M99" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N99" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="N99" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="O99" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P99" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B100" s="7" t="b">
         <v>1</v>
@@ -4698,7 +4803,7 @@
         <v>151.30000000000001</v>
       </c>
       <c r="K100" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L100" s="7"/>
       <c r="M100" s="7"/>
@@ -4707,7 +4812,7 @@
     </row>
     <row r="101" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B101" s="7" t="b">
         <v>1</v>
@@ -4725,27 +4830,27 @@
         <v>207</v>
       </c>
       <c r="K101" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L101" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M101" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N101" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="N101" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="O101" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P101" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B102" s="7" t="b">
         <v>1</v>
@@ -4763,7 +4868,7 @@
         <v>143.65</v>
       </c>
       <c r="K102" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L102" s="7"/>
       <c r="M102" s="7"/>
@@ -4772,7 +4877,7 @@
     </row>
     <row r="103" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B103" s="7" t="b">
         <v>1</v>
@@ -4790,27 +4895,27 @@
         <v>233</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L103" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M103" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N103" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="N103" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="O103" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P103" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B104" s="7" t="b">
         <v>1</v>
@@ -4828,7 +4933,7 @@
         <v>152.36670000000001</v>
       </c>
       <c r="K104" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L104" s="7"/>
       <c r="M104" s="7"/>
@@ -4837,7 +4942,7 @@
     </row>
     <row r="105" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B105" s="7" t="b">
         <v>1</v>
@@ -4855,27 +4960,27 @@
         <v>152.80000000000001</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L105" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M105" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N105" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O105" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P105" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B106" s="7" t="b">
         <v>1</v>
@@ -4893,19 +4998,19 @@
         <v>150.4</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L106" s="7"/>
       <c r="M106" s="7"/>
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
       <c r="P106" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B107" s="7" t="b">
         <v>1</v>
@@ -4923,19 +5028,19 @@
         <v>135.30000000000001</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L107" s="7"/>
       <c r="M107" s="7"/>
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
       <c r="P107" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B108" s="7" t="b">
         <v>1</v>
@@ -4953,19 +5058,19 @@
         <v>135.30000000000001</v>
       </c>
       <c r="K108" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L108" s="7"/>
       <c r="M108" s="7"/>
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
       <c r="P108" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B109" s="22" t="b">
         <v>0</v>
@@ -4983,19 +5088,19 @@
         <v>1981.1289999999999</v>
       </c>
       <c r="K109" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L109" s="22"/>
       <c r="M109" s="22"/>
       <c r="N109" s="22"/>
       <c r="O109" s="22"/>
       <c r="P109" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B110" s="7" t="b">
         <v>1</v>
@@ -5013,27 +5118,27 @@
         <v>155</v>
       </c>
       <c r="K110" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L110" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O110" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P110" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B111" s="7" t="b">
         <v>1</v>
@@ -5051,22 +5156,22 @@
         <v>136.69999999999999</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K111" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L111" s="7"/>
       <c r="M111" s="7"/>
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
       <c r="P111" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B112" s="7" t="b">
         <v>1</v>
@@ -5085,27 +5190,27 @@
         <v>150.4</v>
       </c>
       <c r="K112" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L112" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M112" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N112" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="N112" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="O112" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P112" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B113" s="22" t="b">
         <v>0</v>
@@ -5120,19 +5225,19 @@
         <v>37.375</v>
       </c>
       <c r="K113" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L113" s="22"/>
       <c r="M113" s="22"/>
       <c r="N113" s="22"/>
       <c r="O113" s="22"/>
       <c r="P113" s="21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B114" s="7" t="b">
         <v>1</v>
@@ -5150,24 +5255,24 @@
         <v>148</v>
       </c>
       <c r="K114" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L114" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M114" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N114" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="N114" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="O114" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="115" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B115" s="7" t="b">
         <v>1</v>
@@ -5185,19 +5290,19 @@
         <v>148</v>
       </c>
       <c r="K115" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L115" s="7"/>
       <c r="M115" s="7"/>
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
       <c r="P115" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B116" s="7" t="b">
         <v>1</v>
@@ -5215,27 +5320,27 @@
         <v>150.35</v>
       </c>
       <c r="K116" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L116" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M116" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N116" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="N116" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="O116" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P116" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B117" s="22" t="b">
         <v>0</v>
@@ -5250,19 +5355,19 @@
         <v>47.225000000000001</v>
       </c>
       <c r="K117" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L117" s="22"/>
       <c r="M117" s="22"/>
       <c r="N117" s="22"/>
       <c r="O117" s="22"/>
       <c r="P117" s="21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B118" s="7" t="b">
         <v>1</v>
@@ -5280,27 +5385,27 @@
         <v>151.25</v>
       </c>
       <c r="K118" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L118" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M118" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N118" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="N118" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="O118" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P118" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="119" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B119" s="7" t="b">
         <v>1</v>
@@ -5318,22 +5423,22 @@
         <v>145.69999999999999</v>
       </c>
       <c r="K119" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L119" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M119" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N119" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O119" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P119" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -5344,4 +5449,22 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0782A761-298A-0441-BF3E-1BD817385275}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="32"/>
+    <col min="3" max="3" width="11.6640625" style="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding field data from 2025; updates to groundwater processing scripts
- Added 2025 veg survey data: LAI and IRR raw data for early season
- Added new logger ID info for Solinst Leveloggers
- Very minor updates to groundwater processing scripts (for 2018-2024 data)
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/well_dimensions.xlsx
+++ b/data/field_observations/groundwater/well_dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SANDISK_SSD_G40/GoogleDrive/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE1C07E-0731-2B49-8F20-12723415DB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0035F4-BE41-7244-B423-4C4256C634C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="3760" windowWidth="27180" windowHeight="18360" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
+    <workbookView xWindow="-21600" yWindow="18840" windowWidth="21600" windowHeight="18360" xr2:uid="{DA0B070A-68BE-304A-9361-E14C1481DA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="well_dimensions" sheetId="1" r:id="rId1"/>
@@ -1528,8 +1528,8 @@
   <dimension ref="A1:Q119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>